<commit_message>
implemented data conversion validation checks
</commit_message>
<xml_diff>
--- a/column_notes.xlsx
+++ b/column_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Documents/Local_Code_Projects/lending_club/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62525432-F420-6A4E-8217-3101E9808DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A7126-801A-2047-90A1-F595D3E74FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1240" windowWidth="38400" windowHeight="21100" xr2:uid="{E46DAE9B-FFCA-FE48-926A-5CAFF9548FF8}"/>
+    <workbookView xWindow="18000" yWindow="1100" windowWidth="13560" windowHeight="18340" xr2:uid="{E46DAE9B-FFCA-FE48-926A-5CAFF9548FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
log_reg and rand_for with profit
</commit_message>
<xml_diff>
--- a/column_notes.xlsx
+++ b/column_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Documents/Local_Code_Projects/lending_club/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A7126-801A-2047-90A1-F595D3E74FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2122BEF-17E4-5148-A9D6-A3DA5B0B7127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="1100" windowWidth="13560" windowHeight="18340" xr2:uid="{E46DAE9B-FFCA-FE48-926A-5CAFF9548FF8}"/>
+    <workbookView xWindow="360" yWindow="840" windowWidth="34560" windowHeight="20760" xr2:uid="{E46DAE9B-FFCA-FE48-926A-5CAFF9548FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,32 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>Checks - 10,000 unique values, min: 1 and max: 10,000</t>
-  </si>
-  <si>
     <t>Unique identifier for the loan record</t>
   </si>
   <si>
-    <t>Checks - 10,000 unique values, min: 0 and max: 1</t>
-  </si>
-  <si>
     <t>Binary flag for loan outcome (1 = bad/defaulted, 0 = good)</t>
   </si>
   <si>
-    <t>Look into statistical significance of most common values</t>
-  </si>
-  <si>
     <t>Borrower’s job title as provided on the application</t>
   </si>
   <si>
-    <t xml:space="preserve">Ordinal because the 10+ cap makes it not precise and not equally spaced at the top end </t>
-  </si>
-  <si>
     <t>Length of borrower’s employment in months</t>
   </si>
   <si>
@@ -222,45 +210,6 @@
   </si>
   <si>
     <t>policy_code</t>
-  </si>
-  <si>
-    <t>dtype</t>
-  </si>
-  <si>
-    <t>target_dtype</t>
-  </si>
-  <si>
-    <t>data_type</t>
-  </si>
-  <si>
-    <t>int64</t>
-  </si>
-  <si>
-    <t>Discrete</t>
-  </si>
-  <si>
-    <t>Nominal</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Ordinal</t>
-  </si>
-  <si>
-    <t>float64</t>
-  </si>
-  <si>
-    <t>Ratio</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Checks</t>
   </si>
 </sst>
 </file>
@@ -632,451 +581,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF6407E-A3B7-174A-93CD-C43EA89FB4B0}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="62.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>47</v>
       </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="B20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="B22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="B23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="B25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="B26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="B28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="B29" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>